<commit_message>
compiled data by ayo
</commit_message>
<xml_diff>
--- a/DataCompilation/FTLCompilation.xlsx
+++ b/DataCompilation/FTLCompilation.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Larissa\Desktop\C++Project\Husky\Tests\FTL\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25317"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9408"/>
+    <workbookView xWindow="1400" yWindow="-20" windowWidth="27000" windowHeight="17520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,39 +24,42 @@
     <definedName name="ints_times3_2" localSheetId="0">Sheet1!$D$20:$D$25</definedName>
     <definedName name="ints_times3_3" localSheetId="0">Sheet1!$D$28:$D$33</definedName>
     <definedName name="ints_times3_4" localSheetId="0">Sheet1!$D$36:$D$41</definedName>
-    <definedName name="records_times1" localSheetId="0">Sheet1!$J$4:$J$9</definedName>
-    <definedName name="records_times1_1" localSheetId="0">Sheet1!$J$12:$J$17</definedName>
-    <definedName name="records_times1_2" localSheetId="0">Sheet1!$J$20:$J$25</definedName>
-    <definedName name="records_times1_3" localSheetId="0">Sheet1!$J$28:$J$33</definedName>
-    <definedName name="records_times1_4" localSheetId="0">Sheet1!$J$36:$J$41</definedName>
-    <definedName name="records_times2" localSheetId="0">Sheet1!$K$4:$K$9</definedName>
-    <definedName name="records_times2_1" localSheetId="0">Sheet1!$K$12:$K$17</definedName>
-    <definedName name="records_times2_2" localSheetId="0">Sheet1!$K$20:$K$25</definedName>
-    <definedName name="records_times2_3" localSheetId="0">Sheet1!$G$28:$G$33</definedName>
-    <definedName name="records_times2_4" localSheetId="0">Sheet1!$K$28:$K$33</definedName>
-    <definedName name="records_times2_5" localSheetId="0">Sheet1!$K$36:$K$41</definedName>
-    <definedName name="records_times3" localSheetId="0">Sheet1!$L$4:$L$9</definedName>
-    <definedName name="records_times3_1" localSheetId="0">Sheet1!$L$12:$L$17</definedName>
-    <definedName name="records_times3_2" localSheetId="0">Sheet1!$L$20:$L$25</definedName>
-    <definedName name="records_times3_3" localSheetId="0">Sheet1!$L$28:$L$33</definedName>
-    <definedName name="records_times3_4" localSheetId="0">Sheet1!$L$36:$L$41</definedName>
-    <definedName name="strings_times1_1" localSheetId="0">Sheet1!$F$4:$F$9</definedName>
-    <definedName name="strings_times1_2" localSheetId="0">Sheet1!$F$12:$F$17</definedName>
-    <definedName name="strings_times1_3" localSheetId="0">Sheet1!$F$20:$F$25</definedName>
-    <definedName name="strings_times1_4" localSheetId="0">Sheet1!$F$28:$F$33</definedName>
-    <definedName name="strings_times1_5" localSheetId="0">Sheet1!$F$36:$F$41</definedName>
-    <definedName name="strings_times2" localSheetId="0">Sheet1!$G$4:$G$9</definedName>
-    <definedName name="strings_times2_1" localSheetId="0">Sheet1!$G$12:$G$17</definedName>
-    <definedName name="strings_times2_2" localSheetId="0">Sheet1!$G$20:$G$25</definedName>
-    <definedName name="strings_times2_3" localSheetId="0">Sheet1!$G$36:$G$41</definedName>
-    <definedName name="strings_times3" localSheetId="0">Sheet1!$H$4:$H$9</definedName>
-    <definedName name="strings_times3_1" localSheetId="0">Sheet1!$H$12:$H$17</definedName>
-    <definedName name="strings_times3_2" localSheetId="0">Sheet1!$H$20:$H$25</definedName>
-    <definedName name="strings_times3_3" localSheetId="0">Sheet1!$H$28:$H$33</definedName>
-    <definedName name="strings_times3_4" localSheetId="0">Sheet1!$H$36:$H$41</definedName>
+    <definedName name="records_times1" localSheetId="0">Sheet1!$L$4:$L$9</definedName>
+    <definedName name="records_times1_1" localSheetId="0">Sheet1!$L$12:$L$17</definedName>
+    <definedName name="records_times1_2" localSheetId="0">Sheet1!$L$20:$L$25</definedName>
+    <definedName name="records_times1_3" localSheetId="0">Sheet1!$L$28:$L$33</definedName>
+    <definedName name="records_times1_4" localSheetId="0">Sheet1!$L$36:$L$41</definedName>
+    <definedName name="records_times2" localSheetId="0">Sheet1!$M$4:$M$9</definedName>
+    <definedName name="records_times2_1" localSheetId="0">Sheet1!$M$12:$M$17</definedName>
+    <definedName name="records_times2_2" localSheetId="0">Sheet1!$M$20:$M$25</definedName>
+    <definedName name="records_times2_3" localSheetId="0">Sheet1!$H$28:$H$33</definedName>
+    <definedName name="records_times2_4" localSheetId="0">Sheet1!$M$28:$M$33</definedName>
+    <definedName name="records_times2_5" localSheetId="0">Sheet1!$M$36:$M$41</definedName>
+    <definedName name="records_times3" localSheetId="0">Sheet1!$N$4:$N$9</definedName>
+    <definedName name="records_times3_1" localSheetId="0">Sheet1!$N$12:$N$17</definedName>
+    <definedName name="records_times3_2" localSheetId="0">Sheet1!$N$20:$N$25</definedName>
+    <definedName name="records_times3_3" localSheetId="0">Sheet1!$N$28:$N$33</definedName>
+    <definedName name="records_times3_4" localSheetId="0">Sheet1!$N$36:$N$41</definedName>
+    <definedName name="strings_times1_1" localSheetId="0">Sheet1!$G$4:$G$9</definedName>
+    <definedName name="strings_times1_2" localSheetId="0">Sheet1!$G$12:$G$17</definedName>
+    <definedName name="strings_times1_3" localSheetId="0">Sheet1!$G$20:$G$25</definedName>
+    <definedName name="strings_times1_4" localSheetId="0">Sheet1!$G$28:$G$33</definedName>
+    <definedName name="strings_times1_5" localSheetId="0">Sheet1!$G$36:$G$41</definedName>
+    <definedName name="strings_times2" localSheetId="0">Sheet1!$H$4:$H$9</definedName>
+    <definedName name="strings_times2_1" localSheetId="0">Sheet1!$H$12:$H$17</definedName>
+    <definedName name="strings_times2_2" localSheetId="0">Sheet1!$H$20:$H$25</definedName>
+    <definedName name="strings_times2_3" localSheetId="0">Sheet1!$H$36:$H$41</definedName>
+    <definedName name="strings_times3" localSheetId="0">Sheet1!$I$4:$I$9</definedName>
+    <definedName name="strings_times3_1" localSheetId="0">Sheet1!$I$12:$I$17</definedName>
+    <definedName name="strings_times3_2" localSheetId="0">Sheet1!$I$20:$I$25</definedName>
+    <definedName name="strings_times3_3" localSheetId="0">Sheet1!$I$28:$I$33</definedName>
+    <definedName name="strings_times3_4" localSheetId="0">Sheet1!$I$36:$I$41</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -427,7 +425,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="16">
   <si>
     <t>N = 100000</t>
   </si>
@@ -473,17 +471,43 @@
   <si>
     <t>Records</t>
   </si>
+  <si>
+    <t>avg</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -504,13 +528,346 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="167">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="167">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -527,23 +884,23 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="records-times3_4" connectionId="30" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ints-times1_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="strings-times3_3" connectionId="43" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="strings-times1_3" connectionId="33" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="records-times2_3" connectionId="23" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="strings-times2_2" connectionId="38" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="strings-times1_4" connectionId="34" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="strings-times3_2" connectionId="42" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="records-times3_2" connectionId="28" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="records-times1_2" connectionId="17" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
@@ -551,155 +908,155 @@
 </file>
 
 <file path=xl/queryTables/queryTable15.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="records-times1_2" connectionId="17" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="records-times2_4" connectionId="24" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable16.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="strings-times3_2" connectionId="42" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="strings-times1_4" connectionId="34" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable17.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="strings-times2_2" connectionId="38" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="records-times2_3" connectionId="23" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable18.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="strings-times1_3" connectionId="33" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="strings-times3_3" connectionId="43" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable19.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="records-times1_3" connectionId="18" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ints-times3" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="strings-times1_1" connectionId="31" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable21.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ints-times2_2" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable22.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ints-times3_2" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable23.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ints-times1_4" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable24.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ints-times2_3" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable25.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="records-times3_3" connectionId="29" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable26.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ints-times1_5" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable27.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ints-times2_4" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable28.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ints-times3_4" connectionId="14" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable29.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="strings-times1_5" connectionId="35" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ints-times1_2" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable30.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="strings-times2_3" connectionId="39" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable31.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="strings-times3_4" connectionId="44" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable32.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="records-times1_4" connectionId="19" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable33.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="records-times2_5" connectionId="25" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable34.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="records-times3_4" connectionId="30" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable35.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="strings-times3" connectionId="40" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable36.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="records-times1" connectionId="15" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable37.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="records-times2" connectionId="20" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable38.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="records-times3" connectionId="26" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable39.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="strings-times1_2" connectionId="32" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ints-times2_1" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable40.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="strings-times2_1" connectionId="37" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable41.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="strings-times3_1" connectionId="41" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable42.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="records-times1_1" connectionId="16" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable43.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="records-times2_1" connectionId="21" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable44.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="records-times3_1" connectionId="27" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="records-times2_5" connectionId="25" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable20.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="records-times2_1" connectionId="21" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable21.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="records-times1_1" connectionId="16" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable22.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="strings-times3_1" connectionId="41" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable23.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="strings-times2_1" connectionId="37" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable24.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="strings-times1_2" connectionId="32" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable25.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="records-times3" connectionId="26" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable26.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="records-times2" connectionId="20" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable27.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="records-times1" connectionId="15" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable28.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="strings-times3" connectionId="40" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ints-times3_1" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ints-times1_3" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ints-times3_3" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="strings-times2" connectionId="36" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="records-times1_4" connectionId="19" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable30.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="strings-times1_1" connectionId="31" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable31.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ints-times3_4" connectionId="14" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable32.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ints-times2_4" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable33.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ints-times1_5" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable34.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ints-times3_3" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable35.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ints-times2_3" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable36.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ints-times1_4" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable37.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ints-times3_2" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable38.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ints-times2_2" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable39.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ints-times1_3" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="strings-times3_4" connectionId="44" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable40.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ints-times3_1" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable41.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ints-times2_1" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable42.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ints-times1_2" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable43.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ints-times3" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable44.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="ints-times1_1" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="strings-times2_3" connectionId="39" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="strings-times1_5" connectionId="35" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="records-times3_3" connectionId="29" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="records-times2_4" connectionId="24" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="records-times1_3" connectionId="18" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="records-times3_2" connectionId="28" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -745,7 +1102,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -780,7 +1137,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -957,7 +1314,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -965,41 +1322,53 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L41"/>
+  <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
     <col min="2" max="4" width="4" customWidth="1"/>
-    <col min="5" max="5" width="9.44140625" customWidth="1"/>
-    <col min="6" max="8" width="4" customWidth="1"/>
-    <col min="10" max="12" width="4" customWidth="1"/>
+    <col min="5" max="5" width="4" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5" customWidth="1"/>
+    <col min="7" max="9" width="4" customWidth="1"/>
+    <col min="10" max="10" width="4" style="1" customWidth="1"/>
+    <col min="12" max="14" width="4" customWidth="1"/>
+    <col min="15" max="15" width="4" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="F1" t="s">
+    <row r="1" spans="1:15">
+      <c r="G1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>0</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="G3" t="s">
+      <c r="E3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" t="s">
         <v>13</v>
       </c>
-      <c r="K3" t="s">
+      <c r="J3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="O3" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -1012,8 +1381,9 @@
       <c r="D4">
         <v>8</v>
       </c>
-      <c r="F4">
-        <v>41</v>
+      <c r="E4" s="1">
+        <f>AVERAGE(B4:D4)</f>
+        <v>5.666666666666667</v>
       </c>
       <c r="G4">
         <v>41</v>
@@ -1021,17 +1391,28 @@
       <c r="H4">
         <v>41</v>
       </c>
-      <c r="J4">
+      <c r="I4">
+        <v>41</v>
+      </c>
+      <c r="J4" s="1">
+        <f>AVERAGE(G4:I4)</f>
+        <v>41</v>
+      </c>
+      <c r="L4">
         <v>37</v>
       </c>
-      <c r="K4">
+      <c r="M4">
         <v>35</v>
       </c>
-      <c r="L4">
+      <c r="N4">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="O4" s="1">
+        <f>AVERAGE(L4:N4)</f>
+        <v>35.666666666666664</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1044,26 +1425,38 @@
       <c r="D5">
         <v>0</v>
       </c>
-      <c r="F5">
+      <c r="E5" s="1">
+        <f t="shared" ref="E5:E9" si="0">AVERAGE(B5:D5)</f>
+        <v>0</v>
+      </c>
+      <c r="G5">
         <v>8</v>
-      </c>
-      <c r="G5">
-        <v>7</v>
       </c>
       <c r="H5">
         <v>7</v>
       </c>
-      <c r="J5">
-        <v>8</v>
-      </c>
-      <c r="K5">
-        <v>9</v>
+      <c r="I5">
+        <v>7</v>
+      </c>
+      <c r="J5" s="1">
+        <f t="shared" ref="J5:J9" si="1">AVERAGE(G5:I5)</f>
+        <v>7.333333333333333</v>
       </c>
       <c r="L5">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M5">
+        <v>9</v>
+      </c>
+      <c r="N5">
+        <v>8</v>
+      </c>
+      <c r="O5" s="1">
+        <f t="shared" ref="O5:O9" si="2">AVERAGE(L5:N5)</f>
+        <v>8.3333333333333339</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -1076,26 +1469,38 @@
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="F6">
+      <c r="E6" s="1">
+        <f t="shared" si="0"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="G6">
         <v>11</v>
-      </c>
-      <c r="G6">
-        <v>10</v>
       </c>
       <c r="H6">
         <v>10</v>
       </c>
-      <c r="J6">
+      <c r="I6">
         <v>10</v>
       </c>
-      <c r="K6">
-        <v>10</v>
+      <c r="J6" s="1">
+        <f t="shared" si="1"/>
+        <v>10.333333333333334</v>
       </c>
       <c r="L6">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M6">
+        <v>10</v>
+      </c>
+      <c r="N6">
+        <v>10</v>
+      </c>
+      <c r="O6" s="1">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1108,26 +1513,38 @@
       <c r="D7">
         <v>6</v>
       </c>
-      <c r="F7">
+      <c r="E7" s="1">
+        <f t="shared" si="0"/>
+        <v>6.666666666666667</v>
+      </c>
+      <c r="G7">
         <v>47</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>43</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>44</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="1">
+        <f t="shared" si="1"/>
+        <v>44.666666666666664</v>
+      </c>
+      <c r="L7">
         <v>52</v>
       </c>
-      <c r="K7">
+      <c r="M7">
         <v>52</v>
       </c>
-      <c r="L7">
+      <c r="N7">
         <v>49</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="O7" s="1">
+        <f t="shared" si="2"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -1140,26 +1557,38 @@
       <c r="D8">
         <v>5</v>
       </c>
-      <c r="F8">
+      <c r="E8" s="1">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G8">
         <v>34</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>31</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>29</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="1">
+        <f t="shared" si="1"/>
+        <v>31.333333333333332</v>
+      </c>
+      <c r="L8">
         <v>56</v>
       </c>
-      <c r="K8">
+      <c r="M8">
         <v>49</v>
       </c>
-      <c r="L8">
+      <c r="N8">
         <v>48</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="O8" s="1">
+        <f t="shared" si="2"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1172,31 +1601,43 @@
       <c r="D9">
         <v>42</v>
       </c>
-      <c r="F9">
+      <c r="E9" s="1">
+        <f t="shared" si="0"/>
+        <v>45.666666666666664</v>
+      </c>
+      <c r="G9">
         <v>101</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>97</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>95</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="1">
+        <f t="shared" si="1"/>
+        <v>97.666666666666671</v>
+      </c>
+      <c r="L9">
         <v>92</v>
       </c>
-      <c r="K9">
+      <c r="M9">
         <v>78</v>
       </c>
-      <c r="L9">
+      <c r="N9">
         <v>81</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="O9" s="1">
+        <f t="shared" si="2"/>
+        <v>83.666666666666671</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15">
       <c r="A12" t="s">
         <v>1</v>
       </c>
@@ -1209,26 +1650,38 @@
       <c r="D12">
         <v>13</v>
       </c>
-      <c r="F12">
+      <c r="E12" s="1">
+        <f>AVERAGE(B12:D12)</f>
+        <v>13.333333333333334</v>
+      </c>
+      <c r="G12">
         <v>72</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>74</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>79</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="1">
+        <f>AVERAGE(G12:I12)</f>
+        <v>75</v>
+      </c>
+      <c r="L12">
         <v>72</v>
       </c>
-      <c r="K12">
+      <c r="M12">
         <v>71</v>
       </c>
-      <c r="L12">
+      <c r="N12">
         <v>81</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="O12" s="1">
+        <f>AVERAGE(L12:N12)</f>
+        <v>74.666666666666671</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -1241,26 +1694,38 @@
       <c r="D13">
         <v>1</v>
       </c>
-      <c r="F13">
+      <c r="E13" s="1">
+        <f t="shared" ref="E13:E17" si="3">AVERAGE(B13:D13)</f>
+        <v>1</v>
+      </c>
+      <c r="G13">
         <v>16</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>19</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>15</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="1">
+        <f t="shared" ref="J13:J17" si="4">AVERAGE(G13:I13)</f>
+        <v>16.666666666666668</v>
+      </c>
+      <c r="L13">
         <v>21</v>
       </c>
-      <c r="K13">
+      <c r="M13">
         <v>18</v>
       </c>
-      <c r="L13">
+      <c r="N13">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="O13" s="1">
+        <f t="shared" ref="O13:O17" si="5">AVERAGE(L13:N13)</f>
+        <v>18.666666666666668</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" t="s">
         <v>3</v>
       </c>
@@ -1273,26 +1738,38 @@
       <c r="D14">
         <v>3</v>
       </c>
-      <c r="F14">
-        <v>18</v>
+      <c r="E14" s="1">
+        <f t="shared" si="3"/>
+        <v>3.3333333333333335</v>
       </c>
       <c r="G14">
         <v>18</v>
       </c>
       <c r="H14">
+        <v>18</v>
+      </c>
+      <c r="I14">
         <v>23</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="1">
+        <f t="shared" si="4"/>
+        <v>19.666666666666668</v>
+      </c>
+      <c r="L14">
         <v>19</v>
       </c>
-      <c r="K14">
+      <c r="M14">
         <v>19</v>
       </c>
-      <c r="L14">
+      <c r="N14">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="O14" s="1">
+        <f t="shared" si="5"/>
+        <v>19.333333333333332</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -1305,26 +1782,38 @@
       <c r="D15">
         <v>14</v>
       </c>
-      <c r="F15">
+      <c r="E15" s="1">
+        <f t="shared" si="3"/>
+        <v>13.333333333333334</v>
+      </c>
+      <c r="G15">
         <v>85</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>88</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>90</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="1">
+        <f t="shared" si="4"/>
+        <v>87.666666666666671</v>
+      </c>
+      <c r="L15">
         <v>100</v>
       </c>
-      <c r="K15">
+      <c r="M15">
         <v>104</v>
       </c>
-      <c r="L15">
+      <c r="N15">
         <v>102</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="O15" s="1">
+        <f t="shared" si="5"/>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -1337,26 +1826,38 @@
       <c r="D16">
         <v>10</v>
       </c>
-      <c r="F16">
+      <c r="E16" s="1">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="G16">
         <v>64</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>65</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>64</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="1">
+        <f t="shared" si="4"/>
+        <v>64.333333333333329</v>
+      </c>
+      <c r="L16">
         <v>101</v>
       </c>
-      <c r="K16">
+      <c r="M16">
         <v>102</v>
       </c>
-      <c r="L16">
+      <c r="N16">
         <v>100</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="O16" s="1">
+        <f t="shared" si="5"/>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -1369,31 +1870,43 @@
       <c r="D17">
         <v>89</v>
       </c>
-      <c r="F17">
+      <c r="E17" s="1">
+        <f t="shared" si="3"/>
+        <v>93</v>
+      </c>
+      <c r="G17">
         <v>188</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>194</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>178</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="1">
+        <f t="shared" si="4"/>
+        <v>186.66666666666666</v>
+      </c>
+      <c r="L17">
         <v>170</v>
       </c>
-      <c r="K17">
+      <c r="M17">
         <v>171</v>
       </c>
-      <c r="L17">
+      <c r="N17">
         <v>172</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="O17" s="1">
+        <f t="shared" si="5"/>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -1406,26 +1919,38 @@
       <c r="D20">
         <v>14</v>
       </c>
-      <c r="F20">
+      <c r="E20" s="1">
+        <f>AVERAGE(B20:D20)</f>
+        <v>14.666666666666666</v>
+      </c>
+      <c r="G20">
         <v>119</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>125</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>116</v>
       </c>
-      <c r="J20">
+      <c r="J20" s="1">
+        <f>AVERAGE(G20:I20)</f>
+        <v>120</v>
+      </c>
+      <c r="L20">
         <v>117</v>
       </c>
-      <c r="K20">
+      <c r="M20">
         <v>118</v>
       </c>
-      <c r="L20">
+      <c r="N20">
         <v>126</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="O20" s="1">
+        <f>AVERAGE(L20:N20)</f>
+        <v>120.33333333333333</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -1438,26 +1963,38 @@
       <c r="D21">
         <v>1</v>
       </c>
-      <c r="F21">
-        <v>24</v>
+      <c r="E21" s="1">
+        <f t="shared" ref="E21:E25" si="6">AVERAGE(B21:D21)</f>
+        <v>1</v>
       </c>
       <c r="G21">
         <v>24</v>
       </c>
       <c r="H21">
+        <v>24</v>
+      </c>
+      <c r="I21">
         <v>23</v>
       </c>
-      <c r="J21">
+      <c r="J21" s="1">
+        <f t="shared" ref="J21:J25" si="7">AVERAGE(G21:I21)</f>
+        <v>23.666666666666668</v>
+      </c>
+      <c r="L21">
         <v>27</v>
       </c>
-      <c r="K21">
+      <c r="M21">
         <v>27</v>
       </c>
-      <c r="L21">
+      <c r="N21">
         <v>26</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="O21" s="1">
+        <f t="shared" ref="O21:O25" si="8">AVERAGE(L21:N21)</f>
+        <v>26.666666666666668</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
       <c r="A22" t="s">
         <v>3</v>
       </c>
@@ -1470,26 +2007,38 @@
       <c r="D22">
         <v>5</v>
       </c>
-      <c r="F22">
-        <v>27</v>
+      <c r="E22" s="1">
+        <f t="shared" si="6"/>
+        <v>5</v>
       </c>
       <c r="G22">
         <v>27</v>
       </c>
       <c r="H22">
+        <v>27</v>
+      </c>
+      <c r="I22">
         <v>26</v>
       </c>
-      <c r="J22">
+      <c r="J22" s="1">
+        <f t="shared" si="7"/>
+        <v>26.666666666666668</v>
+      </c>
+      <c r="L22">
         <v>31</v>
       </c>
-      <c r="K22">
+      <c r="M22">
         <v>30</v>
       </c>
-      <c r="L22">
+      <c r="N22">
         <v>33</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="O22" s="1">
+        <f t="shared" si="8"/>
+        <v>31.333333333333332</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -1502,26 +2051,38 @@
       <c r="D23">
         <v>21</v>
       </c>
-      <c r="F23">
+      <c r="E23" s="1">
+        <f t="shared" si="6"/>
+        <v>21</v>
+      </c>
+      <c r="G23">
         <v>143</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <v>151</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <v>146</v>
       </c>
-      <c r="J23">
+      <c r="J23" s="1">
+        <f t="shared" si="7"/>
+        <v>146.66666666666666</v>
+      </c>
+      <c r="L23">
         <v>173</v>
       </c>
-      <c r="K23">
+      <c r="M23">
         <v>172</v>
       </c>
-      <c r="L23">
+      <c r="N23">
         <v>169</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="O23" s="1">
+        <f t="shared" si="8"/>
+        <v>171.33333333333334</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -1534,26 +2095,38 @@
       <c r="D24">
         <v>16</v>
       </c>
-      <c r="F24">
+      <c r="E24" s="1">
+        <f t="shared" si="6"/>
+        <v>19</v>
+      </c>
+      <c r="G24">
         <v>99</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>98</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <v>100</v>
       </c>
-      <c r="J24">
+      <c r="J24" s="1">
+        <f t="shared" si="7"/>
+        <v>99</v>
+      </c>
+      <c r="L24">
         <v>165</v>
       </c>
-      <c r="K24">
+      <c r="M24">
         <v>161</v>
       </c>
-      <c r="L24">
+      <c r="N24">
         <v>159</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="O24" s="1">
+        <f t="shared" si="8"/>
+        <v>161.66666666666666</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -1566,31 +2139,43 @@
       <c r="D25">
         <v>137</v>
       </c>
-      <c r="F25">
+      <c r="E25" s="1">
+        <f t="shared" si="6"/>
+        <v>139.33333333333334</v>
+      </c>
+      <c r="G25">
         <v>291</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>289</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <v>284</v>
       </c>
-      <c r="J25">
+      <c r="J25" s="1">
+        <f t="shared" si="7"/>
+        <v>288</v>
+      </c>
+      <c r="L25">
         <v>268</v>
       </c>
-      <c r="K25">
+      <c r="M25">
         <v>260</v>
       </c>
-      <c r="L25">
+      <c r="N25">
         <v>258</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="O25" s="1">
+        <f t="shared" si="8"/>
+        <v>262</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15">
       <c r="A27" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:15">
       <c r="A28" t="s">
         <v>1</v>
       </c>
@@ -1603,26 +2188,38 @@
       <c r="D28">
         <v>18</v>
       </c>
-      <c r="F28">
+      <c r="E28" s="1">
+        <f>AVERAGE(B28:D28)</f>
+        <v>18</v>
+      </c>
+      <c r="G28">
         <v>158</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <v>159</v>
       </c>
-      <c r="H28">
+      <c r="I28">
         <v>147</v>
       </c>
-      <c r="J28">
+      <c r="J28" s="1">
+        <f>AVERAGE(G28:I28)</f>
+        <v>154.66666666666666</v>
+      </c>
+      <c r="L28">
         <v>144</v>
       </c>
-      <c r="K28">
+      <c r="M28">
         <v>159</v>
       </c>
-      <c r="L28">
+      <c r="N28">
         <v>151</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="O28" s="1">
+        <f>AVERAGE(L28:N28)</f>
+        <v>151.33333333333334</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15">
       <c r="A29" t="s">
         <v>2</v>
       </c>
@@ -1635,26 +2232,38 @@
       <c r="D29">
         <v>2</v>
       </c>
-      <c r="F29">
+      <c r="E29" s="1">
+        <f t="shared" ref="E29:E33" si="9">AVERAGE(B29:D29)</f>
+        <v>2</v>
+      </c>
+      <c r="G29">
         <v>30</v>
       </c>
-      <c r="G29">
+      <c r="H29">
         <v>39</v>
       </c>
-      <c r="H29">
+      <c r="I29">
         <v>33</v>
       </c>
-      <c r="J29">
+      <c r="J29" s="1">
+        <f t="shared" ref="J29:J33" si="10">AVERAGE(G29:I29)</f>
         <v>34</v>
       </c>
-      <c r="K29">
+      <c r="L29">
+        <v>34</v>
+      </c>
+      <c r="M29">
         <v>39</v>
       </c>
-      <c r="L29">
+      <c r="N29">
         <v>37</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="O29" s="1">
+        <f t="shared" ref="O29:O33" si="11">AVERAGE(L29:N29)</f>
+        <v>36.666666666666664</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15">
       <c r="A30" t="s">
         <v>3</v>
       </c>
@@ -1667,26 +2276,38 @@
       <c r="D30">
         <v>7</v>
       </c>
-      <c r="F30">
+      <c r="E30" s="1">
+        <f t="shared" si="9"/>
+        <v>7</v>
+      </c>
+      <c r="G30">
         <v>33</v>
       </c>
-      <c r="G30">
+      <c r="H30">
         <v>38</v>
       </c>
-      <c r="H30">
+      <c r="I30">
         <v>36</v>
       </c>
-      <c r="J30">
+      <c r="J30" s="1">
+        <f t="shared" si="10"/>
+        <v>35.666666666666664</v>
+      </c>
+      <c r="L30">
         <v>38</v>
       </c>
-      <c r="K30">
+      <c r="M30">
         <v>38</v>
       </c>
-      <c r="L30">
+      <c r="N30">
         <v>41</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="O30" s="1">
+        <f t="shared" si="11"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15">
       <c r="A31" t="s">
         <v>4</v>
       </c>
@@ -1699,26 +2320,38 @@
       <c r="D31">
         <v>27</v>
       </c>
-      <c r="F31">
+      <c r="E31" s="1">
+        <f t="shared" si="9"/>
+        <v>27.333333333333332</v>
+      </c>
+      <c r="G31">
         <v>178</v>
       </c>
-      <c r="G31">
+      <c r="H31">
         <v>208</v>
       </c>
-      <c r="H31">
+      <c r="I31">
         <v>185</v>
       </c>
-      <c r="J31">
+      <c r="J31" s="1">
+        <f t="shared" si="10"/>
+        <v>190.33333333333334</v>
+      </c>
+      <c r="L31">
         <v>215</v>
       </c>
-      <c r="K31">
+      <c r="M31">
         <v>208</v>
       </c>
-      <c r="L31">
+      <c r="N31">
         <v>208</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="O31" s="1">
+        <f t="shared" si="11"/>
+        <v>210.33333333333334</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -1731,26 +2364,38 @@
       <c r="D32">
         <v>21</v>
       </c>
-      <c r="F32">
+      <c r="E32" s="1">
+        <f t="shared" si="9"/>
+        <v>20.666666666666668</v>
+      </c>
+      <c r="G32">
         <v>132</v>
       </c>
-      <c r="G32">
+      <c r="H32">
         <v>203</v>
       </c>
-      <c r="H32">
+      <c r="I32">
         <v>125</v>
       </c>
-      <c r="J32">
+      <c r="J32" s="1">
+        <f t="shared" si="10"/>
+        <v>153.33333333333334</v>
+      </c>
+      <c r="L32">
         <v>216</v>
       </c>
-      <c r="K32">
+      <c r="M32">
         <v>203</v>
       </c>
-      <c r="L32">
+      <c r="N32">
         <v>212</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="O32" s="1">
+        <f t="shared" si="11"/>
+        <v>210.33333333333334</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15">
       <c r="A33" t="s">
         <v>6</v>
       </c>
@@ -1763,31 +2408,43 @@
       <c r="D33">
         <v>174</v>
       </c>
-      <c r="F33">
+      <c r="E33" s="1">
+        <f t="shared" si="9"/>
+        <v>178</v>
+      </c>
+      <c r="G33">
         <v>376</v>
       </c>
-      <c r="G33">
+      <c r="H33">
         <v>341</v>
       </c>
-      <c r="H33">
+      <c r="I33">
         <v>367</v>
       </c>
-      <c r="J33">
+      <c r="J33" s="1">
+        <f t="shared" si="10"/>
+        <v>361.33333333333331</v>
+      </c>
+      <c r="L33">
         <v>340</v>
       </c>
-      <c r="K33">
+      <c r="M33">
         <v>341</v>
       </c>
-      <c r="L33">
+      <c r="N33">
         <v>350</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="O33" s="1">
+        <f t="shared" si="11"/>
+        <v>343.66666666666669</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
       <c r="A35" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:15">
       <c r="A36" t="s">
         <v>1</v>
       </c>
@@ -1800,26 +2457,38 @@
       <c r="D36">
         <v>24</v>
       </c>
-      <c r="F36">
+      <c r="E36" s="1">
+        <f>AVERAGE(B36:D36)</f>
+        <v>23.333333333333332</v>
+      </c>
+      <c r="G36">
         <v>184</v>
       </c>
-      <c r="G36">
+      <c r="H36">
         <v>212</v>
       </c>
-      <c r="H36">
+      <c r="I36">
         <v>200</v>
       </c>
-      <c r="J36">
+      <c r="J36" s="1">
+        <f>AVERAGE(G36:I36)</f>
+        <v>198.66666666666666</v>
+      </c>
+      <c r="L36">
         <v>181</v>
       </c>
-      <c r="K36">
+      <c r="M36">
         <v>209</v>
       </c>
-      <c r="L36">
+      <c r="N36">
         <v>202</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="O36" s="1">
+        <f>AVERAGE(L36:N36)</f>
+        <v>197.33333333333334</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
       <c r="A37" t="s">
         <v>2</v>
       </c>
@@ -1832,26 +2501,38 @@
       <c r="D37">
         <v>3</v>
       </c>
-      <c r="F37">
+      <c r="E37" s="1">
+        <f t="shared" ref="E37:E41" si="12">AVERAGE(B37:D37)</f>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="G37">
         <v>37</v>
       </c>
-      <c r="G37">
+      <c r="H37">
         <v>46</v>
       </c>
-      <c r="H37">
+      <c r="I37">
         <v>44</v>
       </c>
-      <c r="J37">
+      <c r="J37" s="1">
+        <f t="shared" ref="J37:J41" si="13">AVERAGE(G37:I37)</f>
+        <v>42.333333333333336</v>
+      </c>
+      <c r="L37">
         <v>43</v>
       </c>
-      <c r="K37">
+      <c r="M37">
         <v>48</v>
       </c>
-      <c r="L37">
+      <c r="N37">
         <v>42</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="O37" s="1">
+        <f t="shared" ref="O37:O41" si="14">AVERAGE(L37:N37)</f>
+        <v>44.333333333333336</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15">
       <c r="A38" t="s">
         <v>3</v>
       </c>
@@ -1864,26 +2545,38 @@
       <c r="D38">
         <v>12</v>
       </c>
-      <c r="F38">
+      <c r="E38" s="1">
+        <f t="shared" si="12"/>
+        <v>10</v>
+      </c>
+      <c r="G38">
         <v>42</v>
       </c>
-      <c r="G38">
+      <c r="H38">
         <v>49</v>
       </c>
-      <c r="H38">
+      <c r="I38">
         <v>50</v>
       </c>
-      <c r="J38">
+      <c r="J38" s="1">
+        <f t="shared" si="13"/>
+        <v>47</v>
+      </c>
+      <c r="L38">
         <v>51</v>
       </c>
-      <c r="K38">
+      <c r="M38">
         <v>56</v>
       </c>
-      <c r="L38">
+      <c r="N38">
         <v>54</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="O38" s="1">
+        <f t="shared" si="14"/>
+        <v>53.666666666666664</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15">
       <c r="A39" t="s">
         <v>4</v>
       </c>
@@ -1896,26 +2589,38 @@
       <c r="D39">
         <v>33</v>
       </c>
-      <c r="F39">
+      <c r="E39" s="1">
+        <f t="shared" si="12"/>
+        <v>36</v>
+      </c>
+      <c r="G39">
         <v>222</v>
       </c>
-      <c r="G39">
+      <c r="H39">
         <v>233</v>
       </c>
-      <c r="H39">
+      <c r="I39">
         <v>220</v>
       </c>
-      <c r="J39">
-        <v>254</v>
-      </c>
-      <c r="K39">
-        <v>258</v>
+      <c r="J39" s="1">
+        <f t="shared" si="13"/>
+        <v>225</v>
       </c>
       <c r="L39">
         <v>254</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M39">
+        <v>258</v>
+      </c>
+      <c r="N39">
+        <v>254</v>
+      </c>
+      <c r="O39" s="1">
+        <f t="shared" si="14"/>
+        <v>255.33333333333334</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15">
       <c r="A40" t="s">
         <v>5</v>
       </c>
@@ -1928,26 +2633,38 @@
       <c r="D40">
         <v>25</v>
       </c>
-      <c r="F40">
+      <c r="E40" s="1">
+        <f t="shared" si="12"/>
+        <v>26</v>
+      </c>
+      <c r="G40">
         <v>166</v>
       </c>
-      <c r="G40">
+      <c r="H40">
         <v>159</v>
       </c>
-      <c r="H40">
+      <c r="I40">
         <v>160</v>
       </c>
-      <c r="J40">
+      <c r="J40" s="1">
+        <f>AVERAGE(G40:I40)</f>
+        <v>161.66666666666666</v>
+      </c>
+      <c r="L40">
         <v>266</v>
       </c>
-      <c r="K40">
+      <c r="M40">
         <v>280</v>
       </c>
-      <c r="L40">
+      <c r="N40">
         <v>277</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="O40" s="1">
+        <f t="shared" si="14"/>
+        <v>274.33333333333331</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15">
       <c r="A41" t="s">
         <v>6</v>
       </c>
@@ -1960,27 +2677,44 @@
       <c r="D41">
         <v>221</v>
       </c>
-      <c r="F41">
+      <c r="E41" s="1">
+        <f t="shared" si="12"/>
+        <v>225</v>
+      </c>
+      <c r="G41">
         <v>464</v>
       </c>
-      <c r="G41">
+      <c r="H41">
         <v>522</v>
       </c>
-      <c r="H41">
+      <c r="I41">
         <v>463</v>
       </c>
-      <c r="J41">
+      <c r="J41" s="1">
+        <f>AVERAGE(G41:I41)</f>
+        <v>483</v>
+      </c>
+      <c r="L41">
         <v>418</v>
       </c>
-      <c r="K41">
+      <c r="M41">
         <v>423</v>
       </c>
-      <c r="L41">
+      <c r="N41">
         <v>416</v>
+      </c>
+      <c r="O41" s="1">
+        <f t="shared" si="14"/>
+        <v>419</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>